<commit_message>
now able to run the whole regression suite in one go except JiraId-1206
</commit_message>
<xml_diff>
--- a/target/classes/TestDataParameterization/DataEngine2.xlsx
+++ b/target/classes/TestDataParameterization/DataEngine2.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="107">
   <si>
     <t>Description</t>
   </si>
@@ -223,9 +223,6 @@
     <t>aleje Jerozolimskie 155, Warsaw, Poland</t>
   </si>
   <si>
-    <t>00-401</t>
-  </si>
-  <si>
     <t>Form Submission</t>
   </si>
   <si>
@@ -352,14 +349,13 @@
     <t>closeSimpleAlert</t>
   </si>
   <si>
-    <t>PASS</t>
+    <t>02-326</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -797,17 +793,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="29" defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="3" style="13" width="29.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" style="12" width="36.140625" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="13" width="30.0" collapsed="true"/>
-    <col min="6" max="16384" style="13" width="29.0" collapsed="true"/>
+    <col min="1" max="3" width="29" style="13" collapsed="1"/>
+    <col min="4" max="4" width="36.140625" style="12" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="30" style="13" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="29" style="13" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="28.5">
@@ -830,7 +826,7 @@
         <v>2</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="43.5">
@@ -849,9 +845,7 @@
       <c r="E2" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="F2" t="s">
-        <v>107</v>
-      </c>
+      <c r="F2"/>
     </row>
     <row r="3" spans="1:7" ht="43.5">
       <c r="A3" s="8" t="s">
@@ -869,9 +863,7 @@
       <c r="E3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="F3" t="s">
-        <v>107</v>
-      </c>
+      <c r="F3"/>
     </row>
     <row r="4" spans="1:7" ht="43.5">
       <c r="A4" s="8"/>
@@ -885,13 +877,11 @@
       <c r="E4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F4" t="s">
-        <v>107</v>
-      </c>
+      <c r="F4"/>
     </row>
     <row r="5" spans="1:7" ht="43.5">
       <c r="A5" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>6</v>
@@ -1039,7 +1029,7 @@
       <c r="A15" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="31" t="s">
+      <c r="B15" s="5" t="s">
         <v>51</v>
       </c>
       <c r="C15" s="5" t="s">
@@ -1078,48 +1068,48 @@
     </row>
     <row r="18" spans="1:7" ht="29.25">
       <c r="A18" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B18" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="B18" s="31" t="s">
+      <c r="C18" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>68</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>69</v>
       </c>
       <c r="F18"/>
     </row>
     <row r="19" spans="1:7" ht="29.25">
       <c r="A19" s="5"/>
       <c r="B19" s="17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F19"/>
       <c r="G19" s="5"/>
     </row>
     <row r="20" spans="1:7" ht="15">
       <c r="A20" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="31" t="s">
         <v>102</v>
-      </c>
-      <c r="B20" s="31" t="s">
-        <v>103</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="5"/>
       <c r="E20" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F20"/>
     </row>
@@ -1129,7 +1119,7 @@
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F21"/>
     </row>
@@ -1139,7 +1129,7 @@
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F22"/>
     </row>
@@ -1204,15 +1194,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="51.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="51" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1265,14 +1255,14 @@
         <v>63</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>64</v>
+        <v>106</v>
       </c>
       <c r="C4" s="20" t="s">
         <v>60</v>
       </c>
       <c r="D4" s="20" t="str">
         <f>CONCATENATE(B4,C4)</f>
-        <v>00-401a</v>
+        <v>02-326a</v>
       </c>
     </row>
   </sheetData>
@@ -1288,40 +1278,40 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" style="21" width="9.5703125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="21" width="11.140625" collapsed="true"/>
-    <col min="4" max="5" customWidth="true" style="21" width="13.7109375" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" style="21" width="9.7109375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="28" width="14.85546875" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="28" width="9.7109375" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" style="21" width="13.140625" collapsed="true"/>
-    <col min="10" max="14" customWidth="true" style="21" width="11.85546875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" style="21" width="10.0" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" style="21" width="14.85546875" collapsed="true"/>
-    <col min="17" max="16384" style="21" width="9.140625" collapsed="true"/>
+    <col min="1" max="2" width="9.5703125" style="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.140625" style="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="5" width="13.7109375" style="21" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="9.7109375" style="21" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.85546875" style="28" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="9.7109375" style="28" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.140625" style="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="14" width="11.85546875" style="21" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="10" style="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="14.85546875" style="21" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="16384" width="9.140625" style="21" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" s="29" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="D1" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="E1" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="F1" s="29" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" s="26" t="s">
         <v>77</v>
-      </c>
-      <c r="E1" s="29" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" s="29" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="26" t="s">
-        <v>78</v>
       </c>
       <c r="H1" s="26"/>
       <c r="I1" s="25"/>
@@ -1332,30 +1322,30 @@
       <c r="N1" s="22"/>
       <c r="O1" s="22"/>
       <c r="P1" s="22" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:16">
       <c r="A2" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="30" t="s">
-        <v>73</v>
-      </c>
       <c r="C2" s="30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D2" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F2" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="30" t="s">
         <v>97</v>
-      </c>
-      <c r="G2" s="30" t="s">
-        <v>98</v>
       </c>
       <c r="H2" s="18"/>
       <c r="I2" s="9"/>
@@ -1371,25 +1361,25 @@
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="30" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="30" t="s">
-        <v>81</v>
-      </c>
       <c r="C3" s="30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F3" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G3" s="30" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I3" s="9"/>
       <c r="J3" s="20"/>
@@ -1404,25 +1394,25 @@
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" s="30" t="s">
         <v>90</v>
       </c>
-      <c r="B4" s="30" t="s">
-        <v>91</v>
-      </c>
       <c r="C4" s="30" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F4" s="30" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H4" s="27"/>
       <c r="J4" s="20"/>
@@ -1454,14 +1444,14 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="1" max="1" width="13" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">

</xml_diff>